<commit_message>
add chart at home
</commit_message>
<xml_diff>
--- a/WebForecastReport/wwwroot/Template/chart.xlsx
+++ b/WebForecastReport/wwwroot/Template/chart.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="48">
   <si>
     <t>Product</t>
   </si>
@@ -155,12 +155,27 @@
   <si>
     <t>Remain Target</t>
   </si>
+  <si>
+    <t>Pending All</t>
+  </si>
+  <si>
+    <t>Quo.</t>
+  </si>
+  <si>
+    <t>Quo</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>No Go</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,8 +183,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,8 +235,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -393,11 +422,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0" hidden="1"/>
@@ -478,13 +518,40 @@
       <alignment horizontal="center"/>
       <protection locked="0" hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0" hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -883,11 +950,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="396904360"/>
-        <c:axId val="396900832"/>
+        <c:axId val="321725808"/>
+        <c:axId val="256199920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="396904360"/>
+        <c:axId val="321725808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -944,15 +1011,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="396900832"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="256199920"/>
+        <c:crossesAt val="1.0000000000000002E-2"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="396900832"/>
+        <c:axId val="256199920"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -987,6 +1054,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:t>MB</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="out"/>
@@ -1020,7 +1143,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="396904360"/>
+        <c:crossAx val="321725808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1207,6 +1330,35 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
               <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -1214,10 +1366,6 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:separator>, </c:separator>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-              </c:extLst>
             </c:dLbl>
             <c:spPr>
               <a:noFill/>
@@ -1255,6 +1403,7 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
+            <c:separator>, </c:separator>
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
@@ -1302,6 +1451,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1424,11 +1574,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="395870800"/>
-        <c:axId val="395871584"/>
+        <c:axId val="256200312"/>
+        <c:axId val="256201096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="395870800"/>
+        <c:axId val="256200312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1485,15 +1635,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="395871584"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="256201096"/>
+        <c:crossesAt val="1.0000000000000002E-2"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="395871584"/>
+        <c:axId val="256201096"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1528,6 +1678,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:t>MB</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="cross"/>
@@ -1561,7 +1767,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="395870800"/>
+        <c:crossAx val="256200312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1945,11 +2151,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="395871192"/>
-        <c:axId val="395869624"/>
+        <c:axId val="256201488"/>
+        <c:axId val="256205800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="395871192"/>
+        <c:axId val="256201488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2006,15 +2212,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="395869624"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="256205800"/>
+        <c:crossesAt val="1.0000000000000002E-2"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="395869624"/>
+        <c:axId val="256205800"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2049,6 +2255,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:t>MB</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="out"/>
@@ -2082,7 +2344,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="395871192"/>
+        <c:crossAx val="256201488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2469,11 +2731,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="395870408"/>
-        <c:axId val="395871976"/>
+        <c:axId val="256202272"/>
+        <c:axId val="256205016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="395870408"/>
+        <c:axId val="256202272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2530,15 +2792,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="395871976"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="256205016"/>
+        <c:crossesAt val="1.0000000000000002E-2"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="395871976"/>
+        <c:axId val="256205016"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2573,6 +2835,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:t>MB</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="out"/>
@@ -2606,7 +2924,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="395870408"/>
+        <c:crossAx val="256202272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3242,11 +3560,11 @@
         </c:dLbls>
         <c:gapWidth val="50"/>
         <c:overlap val="100"/>
-        <c:axId val="395868056"/>
-        <c:axId val="395872368"/>
+        <c:axId val="256202664"/>
+        <c:axId val="256206192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="395868056"/>
+        <c:axId val="256202664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3302,8 +3620,8 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="395872368"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="256206192"/>
+        <c:crossesAt val="1.0000000000000002E-2"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3311,7 +3629,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="395872368"/>
+        <c:axId val="256206192"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3346,6 +3664,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:t>MB</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="out"/>
@@ -3379,7 +3753,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="395868056"/>
+        <c:crossAx val="256202664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3951,11 +4325,11 @@
         </c:dLbls>
         <c:gapWidth val="50"/>
         <c:overlap val="100"/>
-        <c:axId val="395873152"/>
-        <c:axId val="395868448"/>
+        <c:axId val="256206976"/>
+        <c:axId val="138753464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="395873152"/>
+        <c:axId val="256206976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4012,15 +4386,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="395868448"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="138753464"/>
+        <c:crossesAt val="1.0000000000000002E-2"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="395868448"/>
+        <c:axId val="138753464"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4055,6 +4429,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:t>MB</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="out"/>
@@ -4088,7 +4518,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="395873152"/>
+        <c:crossAx val="256206976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4477,11 +4907,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="395869232"/>
-        <c:axId val="395872760"/>
+        <c:axId val="138756600"/>
+        <c:axId val="138755032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="395869232"/>
+        <c:axId val="138756600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4538,15 +4968,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="395872760"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="138755032"/>
+        <c:crossesAt val="1.0000000000000002E-2"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="395872760"/>
+        <c:axId val="138755032"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4581,6 +5011,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:t>MB</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="out"/>
@@ -4614,7 +5100,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="395869232"/>
+        <c:crossAx val="138756600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8510,8 +8996,8 @@
       <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
@@ -8568,16 +9054,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>19049</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>571498</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>285749</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8601,15 +9087,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>447674</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:colOff>485773</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8633,15 +9119,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>103</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8664,16 +9150,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>104</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8696,16 +9182,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>171451</xdr:rowOff>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8994,8 +9480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T59" sqref="T59"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9016,23 +9502,23 @@
   <sheetData>
     <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="27"/>
-      <c r="F2" s="25" t="s">
+      <c r="C2" s="34"/>
+      <c r="D2" s="35"/>
+      <c r="F2" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
-      <c r="J2" s="34" t="s">
+      <c r="G2" s="34"/>
+      <c r="H2" s="35"/>
+      <c r="J2" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="36"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="44"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
@@ -9134,16 +9620,16 @@
       <c r="N7" s="11"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="30"/>
-      <c r="F8" s="28" t="s">
+      <c r="C8" s="37"/>
+      <c r="D8" s="38"/>
+      <c r="F8" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="29"/>
-      <c r="H8" s="30"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="38"/>
       <c r="J8" s="2"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8">
@@ -9231,13 +9717,13 @@
       <c r="F13" s="12"/>
       <c r="G13" s="20"/>
       <c r="H13" s="13"/>
-      <c r="J13" s="31" t="s">
+      <c r="J13" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="33"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="41"/>
     </row>
     <row r="14" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14" t="s">
@@ -9281,16 +9767,16 @@
       <c r="N16" s="9"/>
     </row>
     <row r="17" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="27"/>
-      <c r="F17" s="25" t="s">
+      <c r="C17" s="34"/>
+      <c r="D17" s="35"/>
+      <c r="F17" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="26"/>
-      <c r="H17" s="27"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="35"/>
       <c r="J17" s="12" t="s">
         <v>30</v>
       </c>
@@ -9371,13 +9857,13 @@
       </c>
       <c r="G21" s="8"/>
       <c r="H21" s="9"/>
-      <c r="J21" s="34" t="s">
+      <c r="J21" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="35"/>
-      <c r="N21" s="36"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="44"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
@@ -9400,17 +9886,17 @@
       <c r="N22" s="6"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="29"/>
-      <c r="D23" s="30"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="38"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="28" t="s">
+      <c r="F23" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="G23" s="29"/>
-      <c r="H23" s="30"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="38"/>
       <c r="J23" s="7" t="s">
         <v>0</v>
       </c>
@@ -9483,7 +9969,7 @@
       <c r="D27" s="13"/>
       <c r="E27" s="3"/>
       <c r="F27" s="12"/>
-      <c r="G27" s="23"/>
+      <c r="G27" s="28"/>
       <c r="H27" s="13"/>
       <c r="J27" s="2"/>
       <c r="K27" s="8"/>
@@ -9493,14 +9979,14 @@
       <c r="M27" s="10"/>
       <c r="N27" s="13"/>
     </row>
-    <row r="28" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="12"/>
       <c r="C28" s="20"/>
       <c r="D28" s="13"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="16"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="13"/>
       <c r="J28" s="12"/>
       <c r="K28" s="10"/>
       <c r="L28" s="10"/>
@@ -9513,7 +9999,7 @@
       <c r="D29" s="16"/>
       <c r="E29" s="3"/>
       <c r="F29" s="14"/>
-      <c r="G29" s="24"/>
+      <c r="G29" s="27"/>
       <c r="H29" s="16"/>
       <c r="J29" s="7" t="s">
         <v>28</v>
@@ -9543,18 +10029,18 @@
       <c r="N31" s="13"/>
     </row>
     <row r="32" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="25" t="s">
+      <c r="B32" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="26"/>
-      <c r="D32" s="27"/>
-      <c r="J32" s="31" t="s">
+      <c r="C32" s="34"/>
+      <c r="D32" s="35"/>
+      <c r="J32" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="K32" s="32"/>
-      <c r="L32" s="32"/>
-      <c r="M32" s="32"/>
-      <c r="N32" s="33"/>
+      <c r="K32" s="40"/>
+      <c r="L32" s="40"/>
+      <c r="M32" s="40"/>
+      <c r="N32" s="41"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
@@ -9618,7 +10104,7 @@
       <c r="K36" s="8"/>
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
-      <c r="N36" s="9"/>
+      <c r="N36" s="30"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
@@ -9629,21 +10115,21 @@
       </c>
       <c r="K37" s="8"/>
       <c r="L37" s="5"/>
-      <c r="N37" s="9"/>
+      <c r="N37" s="30"/>
     </row>
     <row r="38" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="28" t="s">
+      <c r="B38" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="29"/>
-      <c r="D38" s="30"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="38"/>
       <c r="J38" s="14" t="s">
         <v>31</v>
       </c>
       <c r="K38" s="15"/>
       <c r="L38" s="17"/>
       <c r="M38" s="17"/>
-      <c r="N38" s="18"/>
+      <c r="N38" s="31"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B39" s="12" t="s">
@@ -9711,15 +10197,623 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="F28:AA126"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="28" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="G28" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="H28" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="I28" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="J28" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="U28" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="V28" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="W28" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="X28" s="26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="F29" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="G29" s="23">
+        <f>'raw data'!C4</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="23">
+        <f>'raw data'!C9</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="23">
+        <f>'raw data'!D4</f>
+        <v>0</v>
+      </c>
+      <c r="J29" s="23">
+        <f>'raw data'!C10</f>
+        <v>0</v>
+      </c>
+      <c r="T29" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="U29" s="23">
+        <f>'raw data'!G4</f>
+        <v>0</v>
+      </c>
+      <c r="V29" s="23">
+        <f>'raw data'!G9</f>
+        <v>0</v>
+      </c>
+      <c r="W29" s="23">
+        <f>'raw data'!H4</f>
+        <v>0</v>
+      </c>
+      <c r="X29" s="23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="F30" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="G30" s="23">
+        <f>'raw data'!C5</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="23">
+        <f>'raw data'!C11</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="23">
+        <f>'raw data'!D5</f>
+        <v>0</v>
+      </c>
+      <c r="J30" s="23">
+        <f>'raw data'!C12</f>
+        <v>0</v>
+      </c>
+      <c r="T30" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="U30" s="23">
+        <f>'raw data'!G5</f>
+        <v>0</v>
+      </c>
+      <c r="V30" s="23">
+        <f>'raw data'!G10</f>
+        <v>0</v>
+      </c>
+      <c r="W30" s="23">
+        <f>'raw data'!H5</f>
+        <v>0</v>
+      </c>
+      <c r="X30" s="23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="F31" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="G31" s="23">
+        <f>'raw data'!C6</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="23">
+        <f>'raw data'!C13</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="23">
+        <f>'raw data'!D6</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="23">
+        <f>'raw data'!C14</f>
+        <v>0</v>
+      </c>
+      <c r="T31" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="U31" s="23">
+        <f>'raw data'!G6</f>
+        <v>0</v>
+      </c>
+      <c r="V31" s="23">
+        <f>'raw data'!G11</f>
+        <v>0</v>
+      </c>
+      <c r="W31" s="23">
+        <f>'raw data'!H6</f>
+        <v>0</v>
+      </c>
+      <c r="X31" s="23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="58" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="G58" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H58" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="I58" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="J58" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="U58" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="V58" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="W58" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="X58" s="26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="59" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="F59" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="G59" s="23">
+        <f>'raw data'!C19</f>
+        <v>0</v>
+      </c>
+      <c r="H59" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="I59" s="23">
+        <f>'raw data'!D19</f>
+        <v>0</v>
+      </c>
+      <c r="J59" s="23">
+        <f>'raw data'!C24</f>
+        <v>0</v>
+      </c>
+      <c r="T59" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="U59" s="23">
+        <f>'raw data'!G19</f>
+        <v>0</v>
+      </c>
+      <c r="V59" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="W59" s="23">
+        <f>'raw data'!H19</f>
+        <v>0</v>
+      </c>
+      <c r="X59" s="23">
+        <f>'raw data'!G24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="F60" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="G60" s="23">
+        <f>'raw data'!C20</f>
+        <v>0</v>
+      </c>
+      <c r="H60" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="I60" s="23">
+        <f>'raw data'!D20</f>
+        <v>0</v>
+      </c>
+      <c r="J60" s="23">
+        <f>'raw data'!C25</f>
+        <v>0</v>
+      </c>
+      <c r="T60" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="U60" s="23">
+        <f>'raw data'!G20</f>
+        <v>0</v>
+      </c>
+      <c r="V60" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="W60" s="23">
+        <f>'raw data'!H20</f>
+        <v>0</v>
+      </c>
+      <c r="X60" s="23">
+        <f>'raw data'!G25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="F61" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="G61" s="23">
+        <f>'raw data'!C21</f>
+        <v>0</v>
+      </c>
+      <c r="H61" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="I61" s="23">
+        <f>'raw data'!D21</f>
+        <v>0</v>
+      </c>
+      <c r="J61" s="23">
+        <f>'raw data'!C26</f>
+        <v>0</v>
+      </c>
+      <c r="T61" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="U61" s="23">
+        <f>'raw data'!G21</f>
+        <v>0</v>
+      </c>
+      <c r="V61" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="W61" s="23">
+        <f>'raw data'!H21</f>
+        <v>0</v>
+      </c>
+      <c r="X61" s="23">
+        <f>'raw data'!G26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="G90" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="H90" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="I90" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J90" s="26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="91" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F91" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="G91" s="23">
+        <f>'raw data'!C34</f>
+        <v>0</v>
+      </c>
+      <c r="H91" s="23">
+        <f>'raw data'!C39</f>
+        <v>0</v>
+      </c>
+      <c r="I91" s="23">
+        <f>'raw data'!D34</f>
+        <v>0</v>
+      </c>
+      <c r="J91" s="23">
+        <f>'raw data'!C40</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F92" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="G92" s="23">
+        <f>'raw data'!C35</f>
+        <v>0</v>
+      </c>
+      <c r="H92" s="23">
+        <f>'raw data'!C41</f>
+        <v>0</v>
+      </c>
+      <c r="I92" s="23">
+        <f>'raw data'!D35</f>
+        <v>0</v>
+      </c>
+      <c r="J92" s="23">
+        <f>'raw data'!C42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F93" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="G93" s="23">
+        <f>'raw data'!C36</f>
+        <v>0</v>
+      </c>
+      <c r="H93" s="23">
+        <f>'raw data'!C43</f>
+        <v>0</v>
+      </c>
+      <c r="I93" s="23">
+        <f>'raw data'!D36</f>
+        <v>0</v>
+      </c>
+      <c r="J93" s="23">
+        <f>'raw data'!C44</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="G123" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="H123" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="I123" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J123" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="K123" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="L123" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="T123" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="U123" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="V123" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="W123" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="X123" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y123" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z123" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA123" s="26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="124" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F124" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="G124" s="23">
+        <f>'raw data'!K23</f>
+        <v>0</v>
+      </c>
+      <c r="H124" s="23">
+        <f>'raw data'!K33</f>
+        <v>0</v>
+      </c>
+      <c r="I124" s="23">
+        <f>'raw data'!L23</f>
+        <v>0</v>
+      </c>
+      <c r="J124" s="23">
+        <f>'raw data'!K34</f>
+        <v>0</v>
+      </c>
+      <c r="K124" s="23">
+        <f>'raw data'!M24</f>
+        <v>0</v>
+      </c>
+      <c r="L124" s="23">
+        <f>'raw data'!N33</f>
+        <v>0</v>
+      </c>
+      <c r="S124" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="T124" s="23">
+        <f>'raw data'!K4</f>
+        <v>0</v>
+      </c>
+      <c r="U124" s="23">
+        <f>'raw data'!K14</f>
+        <v>0</v>
+      </c>
+      <c r="V124" s="23">
+        <f>'raw data'!L4</f>
+        <v>0</v>
+      </c>
+      <c r="W124" s="23">
+        <f>'raw data'!K15</f>
+        <v>0</v>
+      </c>
+      <c r="X124" s="32">
+        <f>'raw data'!M5</f>
+        <v>0</v>
+      </c>
+      <c r="Y124" s="32">
+        <f>'raw data'!N14</f>
+        <v>0</v>
+      </c>
+      <c r="Z124" s="32">
+        <f>'raw data'!N5</f>
+        <v>0</v>
+      </c>
+      <c r="AA124" s="32">
+        <f>'raw data'!N15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F125" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="G125" s="23">
+        <f>'raw data'!K26</f>
+        <v>0</v>
+      </c>
+      <c r="H125" s="23">
+        <f>'raw data'!K35</f>
+        <v>0</v>
+      </c>
+      <c r="I125" s="23">
+        <f>'raw data'!L26</f>
+        <v>0</v>
+      </c>
+      <c r="J125" s="23">
+        <f>'raw data'!K36</f>
+        <v>0</v>
+      </c>
+      <c r="K125" s="23">
+        <f>'raw data'!M27</f>
+        <v>0</v>
+      </c>
+      <c r="L125" s="23">
+        <f>'raw data'!N34</f>
+        <v>0</v>
+      </c>
+      <c r="S125" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="T125" s="23">
+        <f>'raw data'!K7</f>
+        <v>0</v>
+      </c>
+      <c r="U125" s="23">
+        <f>'raw data'!K16</f>
+        <v>0</v>
+      </c>
+      <c r="V125" s="23">
+        <f>'raw data'!L7</f>
+        <v>0</v>
+      </c>
+      <c r="W125" s="23">
+        <f>'raw data'!K17</f>
+        <v>0</v>
+      </c>
+      <c r="X125" s="32">
+        <f>'raw data'!M8</f>
+        <v>0</v>
+      </c>
+      <c r="Y125" s="32">
+        <f>'raw data'!N16</f>
+        <v>0</v>
+      </c>
+      <c r="Z125" s="32">
+        <f>'raw data'!N8</f>
+        <v>0</v>
+      </c>
+      <c r="AA125" s="32">
+        <f>'raw data'!N17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F126" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="G126" s="23">
+        <f>'raw data'!K29</f>
+        <v>0</v>
+      </c>
+      <c r="H126" s="23">
+        <f>'raw data'!K37</f>
+        <v>0</v>
+      </c>
+      <c r="I126" s="23">
+        <f>'raw data'!L29</f>
+        <v>0</v>
+      </c>
+      <c r="J126" s="23">
+        <f>'raw data'!K38</f>
+        <v>0</v>
+      </c>
+      <c r="K126" s="23">
+        <f>'raw data'!M30</f>
+        <v>0</v>
+      </c>
+      <c r="L126" s="23">
+        <f>'raw data'!N35</f>
+        <v>0</v>
+      </c>
+      <c r="S126" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="T126" s="23">
+        <f>'raw data'!K10</f>
+        <v>0</v>
+      </c>
+      <c r="U126" s="23">
+        <f>'raw data'!K18</f>
+        <v>0</v>
+      </c>
+      <c r="V126" s="23">
+        <f>'raw data'!L10</f>
+        <v>0</v>
+      </c>
+      <c r="W126" s="23">
+        <f>'raw data'!K19</f>
+        <v>0</v>
+      </c>
+      <c r="X126" s="32">
+        <f>'raw data'!M11</f>
+        <v>0</v>
+      </c>
+      <c r="Y126" s="32">
+        <f>'raw data'!N18</f>
+        <v>0</v>
+      </c>
+      <c r="Z126" s="32">
+        <f>'raw data'!N11</f>
+        <v>0</v>
+      </c>
+      <c r="AA126" s="32">
+        <f>'raw data'!N19</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>